<commit_message>
rectified algo in test1 but results similar,hence updated algo in test2
</commit_message>
<xml_diff>
--- a/data/explicit/company_keyword.xlsx
+++ b/data/explicit/company_keyword.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="570" windowWidth="14055" windowHeight="4050"/>
+    <workbookView xWindow="600" yWindow="570" windowWidth="14055" windowHeight="4050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
   <si>
     <t>company</t>
   </si>
@@ -145,9 +146,6 @@
     <t>YESBANK,Yes bank,Avi,Rana Kapoor</t>
   </si>
   <si>
-    <t>OTHERS</t>
-  </si>
-  <si>
     <t>AIRTL</t>
   </si>
   <si>
@@ -199,9 +197,6 @@
     <t>Hero Motocorp,HEROMOTOCO,Hero Honda,Brijmohan Lall Munjal,Pawan Munjal,Hero Cycles</t>
   </si>
   <si>
-    <t>mopng,Ministry of Petroleum and Natural Gas,mop&amp;ng,natural gas,petroleum,energy sector,powermin,Ministry of Energy sources,Ministry of New and Renewable Energy,MNRE,Ministry of Power,meity,information technology,I.T.,IT Industry,ITes,banking,finance,financial services,Reserve Bank of India,RBI,R.B.I.,banking system,banking structure,finmin,Ministry of Finance, Department of Financial Services, Pharmaceuticals, Automobile, Automotive</t>
-  </si>
-  <si>
     <t>Mahindra,M&amp;M,Mahindra and Mahindra Limited,Mahindra Group,Anand Mahindra,Pawan Goenka</t>
   </si>
   <si>
@@ -235,19 +230,112 @@
     <t>banking,finance,financial services,Reserve Bank of India,RBI,R.B.I.,banking system,banking structure,finmin,Ministry of Finance, Department of Financial Services</t>
   </si>
   <si>
-    <t>meity,information technology,I.T.,IT Industry,Ites</t>
-  </si>
-  <si>
     <t>mopng,Ministry of Petroleum and Natural Gas,mop&amp;ng,natural gas,petroleum,energy sector,powermin,Ministry of Energy sources,Ministry of New and Renewable Energy,MNRE,Ministry of Power</t>
   </si>
   <si>
-    <t>Telecom,Telecommunication,Ministry of Communication and Information Technology,Department of Telecommunications,</t>
-  </si>
-  <si>
     <t>Pharmaceutical,medicine,drugs</t>
   </si>
   <si>
     <t>Automobile</t>
+  </si>
+  <si>
+    <t>competitors</t>
+  </si>
+  <si>
+    <t>HCL,TM,WIP,TCS</t>
+  </si>
+  <si>
+    <t>INFO,TM,WIP,TCS</t>
+  </si>
+  <si>
+    <t>INFO,HCL,WIP,TCS</t>
+  </si>
+  <si>
+    <t>INFO,HCL,TM,TCS</t>
+  </si>
+  <si>
+    <t>BPCL,GAIL,NTPC,ONGC,PG,TP</t>
+  </si>
+  <si>
+    <t>BPCL,GAIL,NTPC,ONGC,REL,TP</t>
+  </si>
+  <si>
+    <t>BPCL,GAIL,NTPC,PG,REL,TP</t>
+  </si>
+  <si>
+    <t>BPCL,GAIL,ONGC,PG,REL,TP</t>
+  </si>
+  <si>
+    <t>BPCL,NTPC,ONGC,PG,REL,TP</t>
+  </si>
+  <si>
+    <t>GAIL,NTPC,ONGC,PG,REL,TP</t>
+  </si>
+  <si>
+    <t>BPCL,GAIL,NTPC,ONGC,PG,REL</t>
+  </si>
+  <si>
+    <t>AX,BOB,HDFC,HDFCB,ICICI,ININ,KMB,SBI</t>
+  </si>
+  <si>
+    <t>AX,BOB,HDFC,HDFCB,ICICI,ININ,KMB,YB</t>
+  </si>
+  <si>
+    <t>AX,BOB,HDFC,HDFCB,ICICI,ININ,SBI,YB</t>
+  </si>
+  <si>
+    <t>AX,BOB,HDFC,HDFCB,ICICI,KMB,SBI,YB</t>
+  </si>
+  <si>
+    <t>AX,BOB,HDFC,HDFCB,ININ,KMB,SBI,YB</t>
+  </si>
+  <si>
+    <t>AX,BOB,ICICI,ININ,KMB,SBI,YB</t>
+  </si>
+  <si>
+    <t>AX,HDFC,HDFCB,ICICI,ININ,KMB,SBI,YB</t>
+  </si>
+  <si>
+    <t>BOB,HDFC,HDFCB,ICICI,ININ,KMB,SBI,YB</t>
+  </si>
+  <si>
+    <t>LUPIN,SUN</t>
+  </si>
+  <si>
+    <t>CIPLA,SUN</t>
+  </si>
+  <si>
+    <t>LUPIN,CIPLA</t>
+  </si>
+  <si>
+    <t>HERO,MM,MAR,TATAM</t>
+  </si>
+  <si>
+    <t>BAJAJ,MM,MAR,TATAM</t>
+  </si>
+  <si>
+    <t>BAJAJ,MAR,TATAM,HERO</t>
+  </si>
+  <si>
+    <t>BAJAJ,MM,TATAM,HERO</t>
+  </si>
+  <si>
+    <t>BAJAJ,MM,MAR,HERO</t>
+  </si>
+  <si>
+    <t>Telecom,Telecommunication,Department of Telecommunications</t>
+  </si>
+  <si>
+    <t>IDEA,REL</t>
+  </si>
+  <si>
+    <t>AIRTL,REL</t>
+  </si>
+  <si>
+    <t>information technology,IT Industry</t>
+  </si>
+  <si>
+    <t>Infosys,HCL,TechMahindra,Wipro,Accenture,Cognizant,HP,Genpact,IBM</t>
   </si>
 </sst>
 </file>
@@ -608,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -712,7 +800,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
@@ -799,15 +887,15 @@
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>61</v>
+      <c r="B23" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -864,7 +952,7 @@
         <v>51</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1">
@@ -872,23 +960,23 @@
         <v>52</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="4" t="s">
         <v>64</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1">
@@ -896,15 +984,15 @@
         <v>67</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1">
@@ -912,27 +1000,293 @@
         <v>68</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="65.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>